<commit_message>
switch to sniffy, added Bluetooth
</commit_message>
<xml_diff>
--- a/arduino/Pinouts.xlsx
+++ b/arduino/Pinouts.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobye\Documents\github\iot-gibbon\arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577A12C6-598E-4913-AAB5-AA4755F4468B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A44805C-FFA4-454D-BF5A-57780E760A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{6679569A-5730-CD45-91B6-FFE39E759821}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{6679569A-5730-CD45-91B6-FFE39E759821}"/>
   </bookViews>
   <sheets>
     <sheet name="LoLin NodeMcu v3 TFT" sheetId="4" r:id="rId1"/>
-    <sheet name="ESP DevKit V4 C - thermal" sheetId="3" r:id="rId2"/>
-    <sheet name="ESP DevKit V4 C" sheetId="1" r:id="rId3"/>
-    <sheet name="LoLin NodeMcu v3" sheetId="2" r:id="rId4"/>
+    <sheet name="  " sheetId="3" r:id="rId2"/>
+    <sheet name="ESP32" sheetId="6" r:id="rId3"/>
+    <sheet name="ESP DevKit V4 C" sheetId="1" r:id="rId4"/>
+    <sheet name="LoLin NodeMcu v3" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="75">
   <si>
     <t>A-E</t>
   </si>
@@ -228,6 +229,42 @@
   </si>
   <si>
     <t>grey</t>
+  </si>
+  <si>
+    <t>GPIO22</t>
+  </si>
+  <si>
+    <t>D22</t>
+  </si>
+  <si>
+    <t>D33</t>
+  </si>
+  <si>
+    <t>GPIO21</t>
+  </si>
+  <si>
+    <t>D21</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>analogue</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>q</t>
   </si>
 </sst>
 </file>
@@ -418,6 +455,102 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6145" name="AutoShape 1" descr="ESP32 Pinout">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79879B1A-9252-D0AC-FCF9-A0EC12630D88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{532CA8B5-5C99-9391-31F1-9109B316DC59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="4173" t="22789" r="33081" b="14572"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7162801" y="0"/>
+          <a:ext cx="8162924" cy="4581526"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -480,7 +613,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1397,7 +1530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E391671-417A-0D48-9FAC-E45A225572C4}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1952,6 +2085,351 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2047EB23-0A7A-41E5-86F2-974C398D3FB5}">
+  <dimension ref="A1:Q31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="P17" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="F25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="F30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F6CCE2-6773-C849-9C29-21AA552C5F1A}">
   <dimension ref="A1:I31"/>
   <sheetViews>
@@ -2458,12 +2936,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341B22F7-C6B2-C849-97C8-27D41426AA8F}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>